<commit_message>
Added corner peck holes. Adjusted position of items: button, USB header. Removed VBAT and D3_CUT from BOM
</commit_message>
<xml_diff>
--- a/AIRU_WEARABLE_BOM_SEEED_STUDIO_v21.xlsx
+++ b/AIRU_WEARABLE_BOM_SEEED_STUDIO_v21.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\grad-school\laboratory\airQualityControl\repository\airu-board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E77CCFDD-9D11-4AD4-8A3B-7F6E0C1C074A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76306F2-73BC-4918-A7BD-8313262B46B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10080" yWindow="10875" windowWidth="27930" windowHeight="15885" xr2:uid="{0376EBE4-EF8E-4CDE-9B25-51A2D0856E21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{0376EBE4-EF8E-4CDE-9B25-51A2D0856E21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$36</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$G$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="168">
   <si>
     <t>Qty</t>
   </si>
@@ -69,18 +69,6 @@
     <t/>
   </si>
   <si>
-    <t>CONN_02-JST-2MM-SMT</t>
-  </si>
-  <si>
-    <t>JST-2-SMD</t>
-  </si>
-  <si>
-    <t>VBAT</t>
-  </si>
-  <si>
-    <t>Multi connection point. Often used as Generic Header-pin footprint for 0.1 inch spaced/style header connections</t>
-  </si>
-  <si>
     <t>SMD-SWITCH-TACTILE-SPST-NO(4P-D6.0MM)</t>
   </si>
   <si>
@@ -243,9 +231,6 @@
     <t>SOD-123</t>
   </si>
   <si>
-    <t>D1, D2, D3_CUT</t>
-  </si>
-  <si>
     <t>304020034</t>
   </si>
   <si>
@@ -559,6 +544,9 @@
   </si>
   <si>
     <t>ESP32-WROOM-32</t>
+  </si>
+  <si>
+    <t>D1, D2</t>
   </si>
 </sst>
 </file>
@@ -606,7 +594,7 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -624,7 +612,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -672,19 +660,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04BB1746-90C4-43EC-8118-6EE481072013}" name="WAirU_BOM_v2" displayName="WAirU_BOM_v2" ref="A1:G36" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:G36" xr:uid="{49AC22A4-BE7D-446F-B751-2C889F516DFE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G36">
-    <sortCondition ref="B1:B36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04BB1746-90C4-43EC-8118-6EE481072013}" name="WAirU_BOM_v2" displayName="WAirU_BOM_v2" ref="A1:G35" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:G35" xr:uid="{49AC22A4-BE7D-446F-B751-2C889F516DFE}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G35">
+    <sortCondition ref="B1:B35"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6ECD4C4E-6FDF-421B-83AA-38A453A243FE}" uniqueName="1" name="Qty" queryTableFieldId="1" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{3BF47A34-1BA7-46F3-96D4-570C6C93997F}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F52EEF0B-9763-440F-AF75-73FF6D172C1F}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{94ECEA88-67AB-45F2-87FE-246156505CF6}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{61FABAF8-AA96-444B-9327-7069E91DE8C0}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{5B277B47-BB16-47B6-AAF7-BD0E5D1EB613}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{B8D8667C-3C98-4DCD-ADBE-A1EB62B489DD}" uniqueName="13" name="MPN" queryTableFieldId="13" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{6ECD4C4E-6FDF-421B-83AA-38A453A243FE}" uniqueName="1" name="Qty" queryTableFieldId="1" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{3BF47A34-1BA7-46F3-96D4-570C6C93997F}" uniqueName="5" name="Parts" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{F52EEF0B-9763-440F-AF75-73FF6D172C1F}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{94ECEA88-67AB-45F2-87FE-246156505CF6}" uniqueName="2" name="Value" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{61FABAF8-AA96-444B-9327-7069E91DE8C0}" uniqueName="3" name="Device" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{5B277B47-BB16-47B6-AAF7-BD0E5D1EB613}" uniqueName="4" name="Package" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{B8D8667C-3C98-4DCD-ADBE-A1EB62B489DD}" uniqueName="13" name="MPN" queryTableFieldId="13" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -987,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8C324D8-7342-42E1-893A-FEE5B6F290B9}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,22 +1023,22 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1058,22 +1046,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1081,22 +1069,22 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1104,22 +1092,22 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1127,22 +1115,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1150,22 +1138,22 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1173,45 +1161,45 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>167</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1219,22 +1207,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1242,22 +1230,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1265,19 +1253,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>7</v>
@@ -1288,22 +1276,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1311,19 +1299,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>7</v>
@@ -1334,19 +1322,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>7</v>
@@ -1357,22 +1345,22 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1380,22 +1368,22 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1403,22 +1391,22 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1426,22 +1414,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1449,22 +1437,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1472,22 +1460,22 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1495,22 +1483,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1518,22 +1506,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1541,22 +1529,22 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1564,22 +1552,22 @@
         <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1587,22 +1575,22 @@
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1610,22 +1598,22 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1633,19 +1621,19 @@
         <v>3</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>7</v>
@@ -1656,19 +1644,19 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>7</v>
@@ -1679,22 +1667,22 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1702,19 +1690,19 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>7</v>
@@ -1725,22 +1713,22 @@
         <v>1</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D32" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1748,19 +1736,19 @@
         <v>1</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>7</v>
@@ -1771,19 +1759,19 @@
         <v>1</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>7</v>
@@ -1794,51 +1782,29 @@
         <v>1</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>1</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>7</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>